<commit_message>
Thêm thông báo khi gen thành công
</commit_message>
<xml_diff>
--- a/template/evaluatePlan_27-11.xlsx
+++ b/template/evaluatePlan_27-11.xlsx
@@ -1,19 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\FilesDemoFW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\NetBeansProjects\GenCodeSwing\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B44301-0A6B-4824-9261-C58B0BBD0E89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{70D298A5-A85A-43E8-A016-247194F61D59}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="EvaluatePlan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet6" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -288,7 +293,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -725,10 +730,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{930CDF10-6B22-46D4-B62D-D325E8ADF552}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
@@ -1388,4 +1393,76 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>